<commit_message>
Update notebook and dataset
</commit_message>
<xml_diff>
--- a/Splitting_of_Purchase/data/split_purchase_data.xlsx
+++ b/Splitting_of_Purchase/data/split_purchase_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wengz\Desktop\ZS_Github\Data_Engineering\Splitting_of_Purchase\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4C5493-5519-4569-89C0-E7D7A6F7BD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1704BB-D41B-4EB9-8AF0-D0FEA3ED8D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>Purchasing Department</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Purchase Order Date</t>
+  </si>
+  <si>
+    <t>PO_10001008</t>
   </si>
 </sst>
 </file>
@@ -384,7 +387,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -582,13 +585,27 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4">
+        <v>44579</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2">
+        <v>6000</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>

</xml_diff>

<commit_message>
updated dataset for split purchase
</commit_message>
<xml_diff>
--- a/Splitting_of_Purchase/data/split_purchase_data.xlsx
+++ b/Splitting_of_Purchase/data/split_purchase_data.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wengz\Desktop\ZS_Github\Data_Engineering\Splitting_of_Purchase\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1704BB-D41B-4EB9-8AF0-D0FEA3ED8D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55132B46-84A4-44F9-8534-59EE8F8653B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PR Document" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PR Document'!$A$1:$G$9</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -45,27 +48,6 @@
     <t>Dept001</t>
   </si>
   <si>
-    <t>Equipment AA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equipment </t>
-  </si>
-  <si>
-    <t>V0001</t>
-  </si>
-  <si>
-    <t>Equipment AB</t>
-  </si>
-  <si>
-    <t>V0002</t>
-  </si>
-  <si>
-    <t>V0003</t>
-  </si>
-  <si>
-    <t>V0004</t>
-  </si>
-  <si>
     <t>Dept002</t>
   </si>
   <si>
@@ -97,6 +79,27 @@
   </si>
   <si>
     <t>PO_10001008</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Stereo System</t>
+  </si>
+  <si>
+    <t>Audio Visual System</t>
+  </si>
+  <si>
+    <t>Vendor_1</t>
+  </si>
+  <si>
+    <t>Vendor_2</t>
+  </si>
+  <si>
+    <t>Vendor_3</t>
+  </si>
+  <si>
+    <t>Vendor_4</t>
   </si>
 </sst>
 </file>
@@ -387,7 +390,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -405,10 +408,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -428,19 +431,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4">
         <v>44573</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G2" s="2">
         <v>2000</v>
@@ -451,19 +454,19 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4">
         <v>44576</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2">
         <v>4000</v>
@@ -474,19 +477,19 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4">
         <v>44575</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2">
         <v>3000</v>
@@ -497,19 +500,19 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C5" s="4">
         <v>44606</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2">
         <v>6000</v>
@@ -520,19 +523,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4">
         <v>44607</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G6" s="2">
         <v>8000</v>
@@ -540,22 +543,22 @@
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="C7" s="4">
         <v>44577</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G7" s="2">
         <v>4000</v>
@@ -563,22 +566,22 @@
     </row>
     <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4">
         <v>44578</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G8" s="2">
         <v>3000</v>
@@ -586,22 +589,22 @@
     </row>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4">
         <v>44579</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G9" s="2">
         <v>6000</v>

</xml_diff>